<commit_message>
[RDM] - v0.4.0 1) can set/get reader power through modbus,default 2300dBm 2) change to 10s interval for reading tags
[MBS] - v0.4.0
1) set/get reader power

[MBS protocol] - v1.0.3
1) set/get reader power
</commit_message>
<xml_diff>
--- a/doc/PTMS_RDM_Modbus_V1.0.3.xlsx
+++ b/doc/PTMS_RDM_Modbus_V1.0.3.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E77A090-F58C-4365-9365-6BA8C4ADDE1F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BB3A01D-ED58-44DF-B08A-826B38047BE7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="协议说明" sheetId="7" r:id="rId1"/>
@@ -881,10 +881,6 @@
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>7/8/2020</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
     <t>V1.0.3</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
@@ -925,27 +921,28 @@
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>Config file Indicator</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>0xAA55---16 tags config, others---3 tags config</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
     <t>黄色填充单元格是与上个版本的区别</t>
     <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reader Power</t>
+  </si>
+  <si>
+    <t>2300</t>
+  </si>
+  <si>
+    <t>读写器读取功率(dBm),2300/3000</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -953,7 +950,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -979,7 +976,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -988,7 +985,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -996,14 +993,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1277,7 +1274,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1305,28 +1301,73 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1335,50 +1376,8 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1845,16 +1844,16 @@
   <dimension ref="B2:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="59.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="59.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3">
       <c r="B2" s="41" t="s">
         <v>252</v>
       </c>
@@ -1862,11 +1861,11 @@
         <v>253</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3">
       <c r="B3" s="41"/>
       <c r="C3" s="43"/>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3">
       <c r="B4" s="41" t="s">
         <v>254</v>
       </c>
@@ -1874,19 +1873,19 @@
         <v>273</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3">
       <c r="B5" s="41" t="s">
         <v>255</v>
       </c>
-      <c r="C5" s="44" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C5" s="78">
+        <v>44048</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3">
       <c r="B6" s="41"/>
       <c r="C6" s="41"/>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:3">
       <c r="B7" s="41" t="s">
         <v>256</v>
       </c>
@@ -1894,7 +1893,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:3">
       <c r="B8" s="41" t="s">
         <v>258</v>
       </c>
@@ -1902,10 +1901,10 @@
         <v>259</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B11" s="51"/>
+    <row r="11" spans="2:3">
+      <c r="B11" s="50"/>
       <c r="C11" s="42" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
   </sheetData>
@@ -1919,32 +1918,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="C4:J25"/>
   <sheetViews>
-    <sheetView topLeftCell="D4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="5" max="5" width="12.44140625" customWidth="1"/>
-    <col min="6" max="6" width="10.109375" customWidth="1"/>
-    <col min="7" max="7" width="36.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.88671875" customWidth="1"/>
-    <col min="9" max="9" width="52.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" customWidth="1"/>
+    <col min="7" max="7" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" customWidth="1"/>
+    <col min="9" max="9" width="52.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15" style="10" customWidth="1"/>
     <col min="13" max="13" width="15" customWidth="1"/>
     <col min="16" max="16" width="14" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:10">
       <c r="E4" s="1" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="5" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:10">
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="3:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:10" ht="21.75" customHeight="1">
       <c r="E6" s="16" t="s">
         <v>5</v>
       </c>
@@ -1964,17 +1963,17 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="3:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E7" s="56">
+    <row r="7" spans="3:10" ht="20.100000000000001" customHeight="1">
+      <c r="E7" s="59">
         <v>1</v>
       </c>
-      <c r="F7" s="54" t="s">
+      <c r="F7" s="65" t="s">
         <v>119</v>
       </c>
-      <c r="G7" s="58" t="s">
+      <c r="G7" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="H7" s="54" t="s">
+      <c r="H7" s="65" t="s">
         <v>3</v>
       </c>
       <c r="I7" s="8" t="s">
@@ -1984,11 +1983,11 @@
         <v>165</v>
       </c>
     </row>
-    <row r="8" spans="3:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E8" s="57"/>
-      <c r="F8" s="55"/>
-      <c r="G8" s="59"/>
-      <c r="H8" s="55"/>
+    <row r="8" spans="3:10" ht="20.100000000000001" customHeight="1">
+      <c r="E8" s="60"/>
+      <c r="F8" s="66"/>
+      <c r="G8" s="64"/>
+      <c r="H8" s="66"/>
       <c r="I8" s="6" t="s">
         <v>19</v>
       </c>
@@ -1996,7 +1995,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="9" spans="3:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:10" ht="20.100000000000001" customHeight="1">
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
       <c r="E9" s="4">
@@ -2018,33 +2017,35 @@
         <v>166</v>
       </c>
     </row>
-    <row r="10" spans="3:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:10" ht="20.100000000000001" customHeight="1">
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
-      <c r="E10" s="78">
+      <c r="E10" s="58">
         <v>3</v>
       </c>
-      <c r="F10" s="51" t="s">
-        <v>283</v>
-      </c>
-      <c r="G10" s="50" t="s">
+      <c r="F10" s="50" t="s">
+        <v>282</v>
+      </c>
+      <c r="G10" s="49" t="s">
         <v>284</v>
       </c>
-      <c r="H10" s="51" t="s">
+      <c r="H10" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="I10" s="52" t="s">
+      <c r="I10" s="51" t="s">
+        <v>286</v>
+      </c>
+      <c r="J10" s="57" t="s">
         <v>285</v>
       </c>
-      <c r="J10" s="77"/>
-    </row>
-    <row r="11" spans="3:10" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="3:10" ht="41.1" customHeight="1">
       <c r="C11" s="9"/>
       <c r="E11" s="4">
         <v>4</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>28</v>
@@ -2059,7 +2060,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="12" spans="3:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:10" ht="20.100000000000001" customHeight="1">
       <c r="E12" s="4">
         <v>5</v>
       </c>
@@ -2077,7 +2078,7 @@
       </c>
       <c r="J12" s="12"/>
     </row>
-    <row r="13" spans="3:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:10" ht="20.100000000000001" customHeight="1">
       <c r="E13" s="4">
         <v>6</v>
       </c>
@@ -2095,7 +2096,7 @@
       </c>
       <c r="J13" s="12"/>
     </row>
-    <row r="14" spans="3:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:10" ht="20.100000000000001" customHeight="1">
       <c r="E14" s="4">
         <v>7</v>
       </c>
@@ -2113,7 +2114,7 @@
       </c>
       <c r="J14" s="12"/>
     </row>
-    <row r="15" spans="3:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:10" ht="20.100000000000001" customHeight="1">
       <c r="E15" s="4">
         <v>8</v>
       </c>
@@ -2131,7 +2132,7 @@
       </c>
       <c r="J15" s="12"/>
     </row>
-    <row r="16" spans="3:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:10" ht="20.100000000000001" customHeight="1">
       <c r="E16" s="4">
         <v>9</v>
       </c>
@@ -2149,7 +2150,7 @@
       </c>
       <c r="J16" s="12"/>
     </row>
-    <row r="17" spans="5:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="5:10" ht="20.100000000000001" customHeight="1">
       <c r="E17" s="4">
         <v>10</v>
       </c>
@@ -2167,7 +2168,7 @@
       </c>
       <c r="J17" s="12"/>
     </row>
-    <row r="18" spans="5:10" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="5:10" ht="58.5" customHeight="1">
       <c r="E18" s="4">
         <v>11</v>
       </c>
@@ -2185,7 +2186,7 @@
       </c>
       <c r="J18" s="12"/>
     </row>
-    <row r="19" spans="5:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="5:10" ht="20.25" customHeight="1">
       <c r="E19" s="4">
         <v>12</v>
       </c>
@@ -2203,17 +2204,17 @@
       </c>
       <c r="J19" s="12"/>
     </row>
-    <row r="20" spans="5:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E20" s="56">
+    <row r="20" spans="5:10" ht="17.25" customHeight="1">
+      <c r="E20" s="59">
         <v>13</v>
       </c>
-      <c r="F20" s="60" t="s">
+      <c r="F20" s="61" t="s">
         <v>133</v>
       </c>
-      <c r="G20" s="58" t="s">
+      <c r="G20" s="63" t="s">
         <v>148</v>
       </c>
-      <c r="H20" s="54" t="s">
+      <c r="H20" s="65" t="s">
         <v>3</v>
       </c>
       <c r="I20" s="8" t="s">
@@ -2223,11 +2224,11 @@
         <v>118</v>
       </c>
     </row>
-    <row r="21" spans="5:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E21" s="57"/>
-      <c r="F21" s="61"/>
-      <c r="G21" s="59"/>
-      <c r="H21" s="55"/>
+    <row r="21" spans="5:10" ht="19.5" customHeight="1">
+      <c r="E21" s="60"/>
+      <c r="F21" s="62"/>
+      <c r="G21" s="64"/>
+      <c r="H21" s="66"/>
       <c r="I21" s="6" t="s">
         <v>159</v>
       </c>
@@ -2235,17 +2236,17 @@
         <v>118</v>
       </c>
     </row>
-    <row r="22" spans="5:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E22" s="56">
+    <row r="22" spans="5:10" ht="13.5" customHeight="1">
+      <c r="E22" s="59">
         <v>14</v>
       </c>
-      <c r="F22" s="60" t="s">
+      <c r="F22" s="61" t="s">
         <v>175</v>
       </c>
-      <c r="G22" s="58" t="s">
+      <c r="G22" s="63" t="s">
         <v>150</v>
       </c>
-      <c r="H22" s="54" t="s">
+      <c r="H22" s="65" t="s">
         <v>3</v>
       </c>
       <c r="I22" s="8" t="s">
@@ -2255,11 +2256,11 @@
         <v>118</v>
       </c>
     </row>
-    <row r="23" spans="5:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E23" s="57"/>
-      <c r="F23" s="61"/>
-      <c r="G23" s="59"/>
-      <c r="H23" s="55"/>
+    <row r="23" spans="5:10" ht="17.25" customHeight="1">
+      <c r="E23" s="60"/>
+      <c r="F23" s="62"/>
+      <c r="G23" s="64"/>
+      <c r="H23" s="66"/>
       <c r="I23" s="6" t="s">
         <v>167</v>
       </c>
@@ -2267,17 +2268,17 @@
         <v>118</v>
       </c>
     </row>
-    <row r="24" spans="5:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E24" s="56">
+    <row r="24" spans="5:10" ht="20.100000000000001" customHeight="1">
+      <c r="E24" s="59">
         <v>15</v>
       </c>
-      <c r="F24" s="60" t="s">
+      <c r="F24" s="61" t="s">
         <v>176</v>
       </c>
-      <c r="G24" s="58" t="s">
+      <c r="G24" s="63" t="s">
         <v>149</v>
       </c>
-      <c r="H24" s="54" t="s">
+      <c r="H24" s="65" t="s">
         <v>3</v>
       </c>
       <c r="I24" s="8" t="s">
@@ -2287,11 +2288,11 @@
         <v>118</v>
       </c>
     </row>
-    <row r="25" spans="5:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E25" s="57"/>
-      <c r="F25" s="61"/>
-      <c r="G25" s="59"/>
-      <c r="H25" s="55"/>
+    <row r="25" spans="5:10" ht="15.75" customHeight="1">
+      <c r="E25" s="60"/>
+      <c r="F25" s="62"/>
+      <c r="G25" s="64"/>
+      <c r="H25" s="66"/>
       <c r="I25" s="6" t="s">
         <v>162</v>
       </c>
@@ -2301,6 +2302,14 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="H20:H21"/>
     <mergeCell ref="E22:E23"/>
     <mergeCell ref="F22:F23"/>
     <mergeCell ref="G22:G23"/>
@@ -2309,14 +2318,6 @@
     <mergeCell ref="F24:F25"/>
     <mergeCell ref="G24:G25"/>
     <mergeCell ref="H24:H25"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="H20:H21"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2328,24 +2329,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="C3:J79"/>
   <sheetViews>
-    <sheetView topLeftCell="A71" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F94" sqref="F94"/>
+    <sheetView topLeftCell="A72" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C112" sqref="C111:C112"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="5" max="5" width="35.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5546875" customWidth="1"/>
-    <col min="7" max="7" width="51.109375" customWidth="1"/>
-    <col min="8" max="8" width="11.88671875" customWidth="1"/>
+    <col min="5" max="5" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" customWidth="1"/>
+    <col min="7" max="7" width="51.140625" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:8">
       <c r="C3" s="1" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:8">
       <c r="C6" s="16" t="s">
         <v>5</v>
       </c>
@@ -2365,17 +2366,17 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="3:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="62">
+    <row r="7" spans="3:8" ht="20.100000000000001" customHeight="1">
+      <c r="C7" s="76">
         <v>1</v>
       </c>
-      <c r="D7" s="64" t="s">
+      <c r="D7" s="67" t="s">
         <v>119</v>
       </c>
-      <c r="E7" s="66" t="s">
+      <c r="E7" s="70" t="s">
         <v>151</v>
       </c>
-      <c r="F7" s="64" t="s">
+      <c r="F7" s="67" t="s">
         <v>3</v>
       </c>
       <c r="G7" s="23" t="s">
@@ -2383,27 +2384,27 @@
       </c>
       <c r="H7" s="11"/>
     </row>
-    <row r="8" spans="3:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="63"/>
-      <c r="D8" s="65"/>
-      <c r="E8" s="67"/>
-      <c r="F8" s="65"/>
+    <row r="8" spans="3:8" ht="20.100000000000001" customHeight="1">
+      <c r="C8" s="77"/>
+      <c r="D8" s="69"/>
+      <c r="E8" s="72"/>
+      <c r="F8" s="69"/>
       <c r="G8" s="24" t="s">
         <v>163</v>
       </c>
       <c r="H8" s="12"/>
     </row>
-    <row r="9" spans="3:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="62">
+    <row r="9" spans="3:8" ht="20.100000000000001" customHeight="1">
+      <c r="C9" s="76">
         <v>2</v>
       </c>
-      <c r="D9" s="64" t="s">
+      <c r="D9" s="67" t="s">
         <v>120</v>
       </c>
-      <c r="E9" s="66" t="s">
+      <c r="E9" s="70" t="s">
         <v>152</v>
       </c>
-      <c r="F9" s="64" t="s">
+      <c r="F9" s="67" t="s">
         <v>3</v>
       </c>
       <c r="G9" s="23" t="s">
@@ -2411,27 +2412,27 @@
       </c>
       <c r="H9" s="11"/>
     </row>
-    <row r="10" spans="3:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="63"/>
-      <c r="D10" s="65"/>
-      <c r="E10" s="67"/>
-      <c r="F10" s="65"/>
+    <row r="10" spans="3:8" ht="20.100000000000001" customHeight="1">
+      <c r="C10" s="77"/>
+      <c r="D10" s="69"/>
+      <c r="E10" s="72"/>
+      <c r="F10" s="69"/>
       <c r="G10" s="24" t="s">
         <v>155</v>
       </c>
       <c r="H10" s="12"/>
     </row>
-    <row r="11" spans="3:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="62">
+    <row r="11" spans="3:8" ht="20.100000000000001" customHeight="1">
+      <c r="C11" s="76">
         <v>3</v>
       </c>
-      <c r="D11" s="64" t="s">
+      <c r="D11" s="67" t="s">
         <v>121</v>
       </c>
-      <c r="E11" s="66" t="s">
+      <c r="E11" s="70" t="s">
         <v>153</v>
       </c>
-      <c r="F11" s="64" t="s">
+      <c r="F11" s="67" t="s">
         <v>265</v>
       </c>
       <c r="G11" s="23" t="s">
@@ -2439,89 +2440,89 @@
       </c>
       <c r="H11" s="11"/>
     </row>
-    <row r="12" spans="3:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="63"/>
-      <c r="D12" s="65"/>
-      <c r="E12" s="67"/>
-      <c r="F12" s="65"/>
+    <row r="12" spans="3:8" ht="20.100000000000001" customHeight="1">
+      <c r="C12" s="77"/>
+      <c r="D12" s="69"/>
+      <c r="E12" s="72"/>
+      <c r="F12" s="69"/>
       <c r="G12" s="24" t="s">
         <v>157</v>
       </c>
       <c r="H12" s="12"/>
     </row>
-    <row r="13" spans="3:8" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:8" ht="43.15" customHeight="1">
       <c r="C13" s="25">
         <v>4</v>
       </c>
-      <c r="D13" s="47" t="s">
+      <c r="D13" s="46" t="s">
         <v>263</v>
       </c>
-      <c r="E13" s="74" t="s">
+      <c r="E13" s="54" t="s">
         <v>261</v>
       </c>
-      <c r="F13" s="75" t="s">
+      <c r="F13" s="55" t="s">
         <v>262</v>
       </c>
-      <c r="G13" s="76" t="s">
+      <c r="G13" s="56" t="s">
         <v>272</v>
       </c>
       <c r="H13" s="12"/>
     </row>
-    <row r="14" spans="3:8" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="46">
+    <row r="14" spans="3:8" ht="52.5" customHeight="1">
+      <c r="C14" s="45">
         <v>5</v>
       </c>
-      <c r="D14" s="47" t="s">
+      <c r="D14" s="46" t="s">
         <v>266</v>
       </c>
-      <c r="E14" s="74" t="s">
+      <c r="E14" s="54" t="s">
         <v>264</v>
       </c>
-      <c r="F14" s="75" t="s">
+      <c r="F14" s="55" t="s">
         <v>265</v>
       </c>
-      <c r="G14" s="76" t="s">
+      <c r="G14" s="56" t="s">
         <v>271</v>
       </c>
       <c r="H14" s="12"/>
     </row>
-    <row r="15" spans="3:8" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="48">
+    <row r="15" spans="3:8" ht="52.5" customHeight="1">
+      <c r="C15" s="47">
         <v>6</v>
       </c>
-      <c r="D15" s="49" t="s">
+      <c r="D15" s="48" t="s">
+        <v>276</v>
+      </c>
+      <c r="E15" s="49" t="s">
         <v>277</v>
       </c>
-      <c r="E15" s="50" t="s">
-        <v>278</v>
-      </c>
-      <c r="F15" s="51" t="s">
+      <c r="F15" s="50" t="s">
         <v>265</v>
       </c>
-      <c r="G15" s="52" t="s">
+      <c r="G15" s="51" t="s">
+        <v>279</v>
+      </c>
+      <c r="H15" s="12"/>
+    </row>
+    <row r="16" spans="3:8" ht="52.5" customHeight="1">
+      <c r="C16" s="45">
+        <v>6</v>
+      </c>
+      <c r="D16" s="48" t="s">
         <v>280</v>
       </c>
-      <c r="H15" s="12"/>
-    </row>
-    <row r="16" spans="3:8" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="46">
-        <v>6</v>
-      </c>
-      <c r="D16" s="49" t="s">
-        <v>281</v>
-      </c>
-      <c r="E16" s="50"/>
-      <c r="F16" s="51" t="s">
+      <c r="E16" s="49"/>
+      <c r="F16" s="50" t="s">
         <v>265</v>
       </c>
-      <c r="G16" s="52" t="s">
+      <c r="G16" s="51" t="s">
         <v>268</v>
       </c>
       <c r="H16" s="12" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="17" spans="3:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:10" ht="27.75" customHeight="1">
       <c r="C17" s="25">
         <v>7</v>
       </c>
@@ -2539,8 +2540,8 @@
       </c>
       <c r="H17" s="12"/>
     </row>
-    <row r="18" spans="3:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C18" s="46">
+    <row r="18" spans="3:10" ht="20.100000000000001" customHeight="1">
+      <c r="C18" s="45">
         <v>8</v>
       </c>
       <c r="D18" s="5" t="s">
@@ -2552,16 +2553,16 @@
       <c r="F18" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="G18" s="53" t="s">
-        <v>279</v>
+      <c r="G18" s="52" t="s">
+        <v>278</v>
       </c>
       <c r="H18" s="12"/>
       <c r="J18" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="19" spans="3:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="46">
+    <row r="19" spans="3:10" ht="20.100000000000001" customHeight="1">
+      <c r="C19" s="45">
         <v>9</v>
       </c>
       <c r="D19" s="5" t="s">
@@ -2581,8 +2582,8 @@
         <v>89</v>
       </c>
     </row>
-    <row r="20" spans="3:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C20" s="46">
+    <row r="20" spans="3:10" ht="20.100000000000001" customHeight="1">
+      <c r="C20" s="45">
         <v>10</v>
       </c>
       <c r="D20" s="5" t="s">
@@ -2599,8 +2600,8 @@
       </c>
       <c r="H20" s="12"/>
     </row>
-    <row r="21" spans="3:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C21" s="46">
+    <row r="21" spans="3:10" ht="20.100000000000001" customHeight="1">
+      <c r="C21" s="45">
         <v>11</v>
       </c>
       <c r="D21" s="5" t="s">
@@ -2617,8 +2618,8 @@
       </c>
       <c r="H21" s="12"/>
     </row>
-    <row r="22" spans="3:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C22" s="46">
+    <row r="22" spans="3:10" ht="20.100000000000001" customHeight="1">
+      <c r="C22" s="45">
         <v>12</v>
       </c>
       <c r="D22" s="5" t="s">
@@ -2635,8 +2636,8 @@
       </c>
       <c r="H22" s="12"/>
     </row>
-    <row r="23" spans="3:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C23" s="46">
+    <row r="23" spans="3:10" ht="20.100000000000001" customHeight="1">
+      <c r="C23" s="45">
         <v>13</v>
       </c>
       <c r="D23" s="5" t="s">
@@ -2653,7 +2654,7 @@
       </c>
       <c r="H23" s="12"/>
     </row>
-    <row r="24" spans="3:10" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:10" ht="48" customHeight="1">
       <c r="C24" s="5">
         <v>14</v>
       </c>
@@ -2671,7 +2672,7 @@
       </c>
       <c r="H24" s="12"/>
     </row>
-    <row r="25" spans="3:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:10" ht="25.5" customHeight="1">
       <c r="C25" s="5">
         <v>15</v>
       </c>
@@ -2689,7 +2690,7 @@
       </c>
       <c r="H25" s="12"/>
     </row>
-    <row r="26" spans="3:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:10" ht="20.100000000000001" customHeight="1">
       <c r="C26" s="5">
         <v>16</v>
       </c>
@@ -2707,7 +2708,7 @@
       </c>
       <c r="H26" s="12"/>
     </row>
-    <row r="27" spans="3:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:10" ht="20.100000000000001" customHeight="1">
       <c r="C27" s="5">
         <v>17</v>
       </c>
@@ -2725,7 +2726,7 @@
       </c>
       <c r="H27" s="12"/>
     </row>
-    <row r="28" spans="3:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:10" ht="20.100000000000001" customHeight="1">
       <c r="C28" s="5">
         <v>18</v>
       </c>
@@ -2743,7 +2744,7 @@
       </c>
       <c r="H28" s="12"/>
     </row>
-    <row r="29" spans="3:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:10" ht="20.100000000000001" customHeight="1">
       <c r="C29" s="5">
         <v>19</v>
       </c>
@@ -2761,7 +2762,7 @@
       </c>
       <c r="H29" s="12"/>
     </row>
-    <row r="30" spans="3:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:10" ht="20.100000000000001" customHeight="1">
       <c r="C30" s="5">
         <v>20</v>
       </c>
@@ -2779,7 +2780,7 @@
       </c>
       <c r="H30" s="12"/>
     </row>
-    <row r="31" spans="3:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:10" ht="20.100000000000001" customHeight="1">
       <c r="C31" s="5">
         <v>21</v>
       </c>
@@ -2797,7 +2798,7 @@
       </c>
       <c r="H31" s="12"/>
     </row>
-    <row r="32" spans="3:10" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:10" ht="41.1" customHeight="1">
       <c r="C32" s="5">
         <v>22</v>
       </c>
@@ -2815,7 +2816,7 @@
       </c>
       <c r="H32" s="12"/>
     </row>
-    <row r="33" spans="3:8" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:8" ht="41.1" customHeight="1">
       <c r="C33" s="5">
         <v>23</v>
       </c>
@@ -2833,7 +2834,7 @@
       </c>
       <c r="H33" s="12"/>
     </row>
-    <row r="34" spans="3:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:8" ht="20.100000000000001" customHeight="1">
       <c r="C34" s="5">
         <v>24</v>
       </c>
@@ -2851,7 +2852,7 @@
       </c>
       <c r="H34" s="12"/>
     </row>
-    <row r="35" spans="3:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:8" ht="20.100000000000001" customHeight="1">
       <c r="C35" s="5">
         <v>25</v>
       </c>
@@ -2869,7 +2870,7 @@
       </c>
       <c r="H35" s="12"/>
     </row>
-    <row r="36" spans="3:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:8" ht="20.100000000000001" customHeight="1">
       <c r="C36" s="5">
         <v>26</v>
       </c>
@@ -2887,7 +2888,7 @@
       </c>
       <c r="H36" s="12"/>
     </row>
-    <row r="37" spans="3:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:8" ht="20.100000000000001" customHeight="1">
       <c r="C37" s="5">
         <v>27</v>
       </c>
@@ -2905,7 +2906,7 @@
       </c>
       <c r="H37" s="12"/>
     </row>
-    <row r="38" spans="3:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:8" ht="20.100000000000001" customHeight="1">
       <c r="C38" s="5">
         <v>28</v>
       </c>
@@ -2923,7 +2924,7 @@
       </c>
       <c r="H38" s="12"/>
     </row>
-    <row r="39" spans="3:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:8" ht="20.100000000000001" customHeight="1">
       <c r="C39" s="5">
         <v>29</v>
       </c>
@@ -2941,7 +2942,7 @@
       </c>
       <c r="H39" s="12"/>
     </row>
-    <row r="40" spans="3:8" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:8" ht="51.75" customHeight="1">
       <c r="C40" s="5">
         <v>30</v>
       </c>
@@ -2959,7 +2960,7 @@
       </c>
       <c r="H40" s="12"/>
     </row>
-    <row r="41" spans="3:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:8" ht="20.100000000000001" customHeight="1">
       <c r="C41" s="5">
         <v>31</v>
       </c>
@@ -2977,295 +2978,295 @@
       </c>
       <c r="H41" s="12"/>
     </row>
-    <row r="42" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C42" s="64">
+    <row r="42" spans="3:8">
+      <c r="C42" s="67">
         <v>32</v>
       </c>
-      <c r="D42" s="64" t="s">
+      <c r="D42" s="67" t="s">
         <v>136</v>
       </c>
-      <c r="E42" s="66" t="s">
+      <c r="E42" s="70" t="s">
         <v>10</v>
       </c>
-      <c r="F42" s="64" t="s">
+      <c r="F42" s="67" t="s">
         <v>9</v>
       </c>
       <c r="G42" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="H42" s="70"/>
-    </row>
-    <row r="43" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="H42" s="73"/>
+    </row>
+    <row r="43" spans="3:8">
       <c r="C43" s="68"/>
       <c r="D43" s="68"/>
-      <c r="E43" s="69"/>
+      <c r="E43" s="71"/>
       <c r="F43" s="68"/>
       <c r="G43" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="H43" s="71"/>
-    </row>
-    <row r="44" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="H43" s="74"/>
+    </row>
+    <row r="44" spans="3:8">
       <c r="C44" s="68"/>
       <c r="D44" s="68"/>
-      <c r="E44" s="69"/>
+      <c r="E44" s="71"/>
       <c r="F44" s="68"/>
       <c r="G44" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="H44" s="71"/>
-    </row>
-    <row r="45" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C45" s="65"/>
-      <c r="D45" s="65"/>
-      <c r="E45" s="67"/>
-      <c r="F45" s="65"/>
+      <c r="H44" s="74"/>
+    </row>
+    <row r="45" spans="3:8">
+      <c r="C45" s="69"/>
+      <c r="D45" s="69"/>
+      <c r="E45" s="72"/>
+      <c r="F45" s="69"/>
       <c r="G45" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="H45" s="72"/>
-    </row>
-    <row r="46" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C46" s="64">
+      <c r="H45" s="75"/>
+    </row>
+    <row r="46" spans="3:8">
+      <c r="C46" s="67">
         <v>33</v>
       </c>
-      <c r="D46" s="64" t="s">
+      <c r="D46" s="67" t="s">
         <v>211</v>
       </c>
-      <c r="E46" s="66" t="s">
+      <c r="E46" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="F46" s="64" t="s">
+      <c r="F46" s="67" t="s">
         <v>9</v>
       </c>
       <c r="G46" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="H46" s="70"/>
-    </row>
-    <row r="47" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="H46" s="73"/>
+    </row>
+    <row r="47" spans="3:8">
       <c r="C47" s="68"/>
       <c r="D47" s="68"/>
-      <c r="E47" s="69"/>
+      <c r="E47" s="71"/>
       <c r="F47" s="68"/>
       <c r="G47" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="H47" s="71"/>
-    </row>
-    <row r="48" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="H47" s="74"/>
+    </row>
+    <row r="48" spans="3:8">
       <c r="C48" s="68"/>
       <c r="D48" s="68"/>
-      <c r="E48" s="69"/>
+      <c r="E48" s="71"/>
       <c r="F48" s="68"/>
       <c r="G48" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="H48" s="71"/>
-    </row>
-    <row r="49" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C49" s="65"/>
-      <c r="D49" s="65"/>
-      <c r="E49" s="67"/>
-      <c r="F49" s="65"/>
+      <c r="H48" s="74"/>
+    </row>
+    <row r="49" spans="3:8">
+      <c r="C49" s="69"/>
+      <c r="D49" s="69"/>
+      <c r="E49" s="72"/>
+      <c r="F49" s="69"/>
       <c r="G49" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="H49" s="72"/>
-    </row>
-    <row r="50" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C50" s="64">
+      <c r="H49" s="75"/>
+    </row>
+    <row r="50" spans="3:8">
+      <c r="C50" s="67">
         <v>34</v>
       </c>
-      <c r="D50" s="64" t="s">
+      <c r="D50" s="67" t="s">
         <v>137</v>
       </c>
-      <c r="E50" s="66" t="s">
+      <c r="E50" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="F50" s="64" t="s">
+      <c r="F50" s="67" t="s">
         <v>9</v>
       </c>
       <c r="G50" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="H50" s="70"/>
-    </row>
-    <row r="51" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="H50" s="73"/>
+    </row>
+    <row r="51" spans="3:8">
       <c r="C51" s="68"/>
       <c r="D51" s="68"/>
-      <c r="E51" s="69"/>
+      <c r="E51" s="71"/>
       <c r="F51" s="68"/>
       <c r="G51" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="H51" s="71"/>
-    </row>
-    <row r="52" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="H51" s="74"/>
+    </row>
+    <row r="52" spans="3:8">
       <c r="C52" s="68"/>
       <c r="D52" s="68"/>
-      <c r="E52" s="69"/>
+      <c r="E52" s="71"/>
       <c r="F52" s="68"/>
       <c r="G52" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="H52" s="71"/>
-    </row>
-    <row r="53" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C53" s="65"/>
-      <c r="D53" s="65"/>
-      <c r="E53" s="67"/>
-      <c r="F53" s="65"/>
+      <c r="H52" s="74"/>
+    </row>
+    <row r="53" spans="3:8">
+      <c r="C53" s="69"/>
+      <c r="D53" s="69"/>
+      <c r="E53" s="72"/>
+      <c r="F53" s="69"/>
       <c r="G53" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="H53" s="72"/>
-    </row>
-    <row r="54" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C54" s="64">
+      <c r="H53" s="75"/>
+    </row>
+    <row r="54" spans="3:8">
+      <c r="C54" s="67">
         <v>35</v>
       </c>
-      <c r="D54" s="64" t="s">
+      <c r="D54" s="67" t="s">
         <v>212</v>
       </c>
-      <c r="E54" s="66" t="s">
+      <c r="E54" s="70" t="s">
         <v>26</v>
       </c>
-      <c r="F54" s="64" t="s">
+      <c r="F54" s="67" t="s">
         <v>9</v>
       </c>
       <c r="G54" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="H54" s="70"/>
-    </row>
-    <row r="55" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="H54" s="73"/>
+    </row>
+    <row r="55" spans="3:8">
       <c r="C55" s="68"/>
       <c r="D55" s="68"/>
-      <c r="E55" s="69"/>
+      <c r="E55" s="71"/>
       <c r="F55" s="68"/>
       <c r="G55" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="H55" s="71"/>
-    </row>
-    <row r="56" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="H55" s="74"/>
+    </row>
+    <row r="56" spans="3:8">
       <c r="C56" s="68"/>
       <c r="D56" s="68"/>
-      <c r="E56" s="69"/>
+      <c r="E56" s="71"/>
       <c r="F56" s="68"/>
       <c r="G56" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="H56" s="71"/>
-    </row>
-    <row r="57" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C57" s="65"/>
-      <c r="D57" s="65"/>
-      <c r="E57" s="67"/>
-      <c r="F57" s="65"/>
+      <c r="H56" s="74"/>
+    </row>
+    <row r="57" spans="3:8">
+      <c r="C57" s="69"/>
+      <c r="D57" s="69"/>
+      <c r="E57" s="72"/>
+      <c r="F57" s="69"/>
       <c r="G57" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="H57" s="72"/>
-    </row>
-    <row r="58" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C58" s="64">
+      <c r="H57" s="75"/>
+    </row>
+    <row r="58" spans="3:8">
+      <c r="C58" s="67">
         <v>36</v>
       </c>
-      <c r="D58" s="64" t="s">
+      <c r="D58" s="67" t="s">
         <v>138</v>
       </c>
-      <c r="E58" s="66" t="s">
+      <c r="E58" s="70" t="s">
         <v>55</v>
       </c>
-      <c r="F58" s="64" t="s">
+      <c r="F58" s="67" t="s">
         <v>9</v>
       </c>
       <c r="G58" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="H58" s="70"/>
-    </row>
-    <row r="59" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="H58" s="73"/>
+    </row>
+    <row r="59" spans="3:8">
       <c r="C59" s="68"/>
       <c r="D59" s="68"/>
-      <c r="E59" s="69"/>
+      <c r="E59" s="71"/>
       <c r="F59" s="68"/>
       <c r="G59" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="H59" s="71"/>
-    </row>
-    <row r="60" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="H59" s="74"/>
+    </row>
+    <row r="60" spans="3:8">
       <c r="C60" s="68"/>
       <c r="D60" s="68"/>
-      <c r="E60" s="69"/>
+      <c r="E60" s="71"/>
       <c r="F60" s="68"/>
       <c r="G60" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="H60" s="71"/>
-    </row>
-    <row r="61" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C61" s="65"/>
-      <c r="D61" s="65"/>
-      <c r="E61" s="67"/>
-      <c r="F61" s="65"/>
+      <c r="H60" s="74"/>
+    </row>
+    <row r="61" spans="3:8">
+      <c r="C61" s="69"/>
+      <c r="D61" s="69"/>
+      <c r="E61" s="72"/>
+      <c r="F61" s="69"/>
       <c r="G61" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="H61" s="72"/>
-    </row>
-    <row r="62" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C62" s="64">
+      <c r="H61" s="75"/>
+    </row>
+    <row r="62" spans="3:8">
+      <c r="C62" s="67">
         <v>37</v>
       </c>
-      <c r="D62" s="64" t="s">
+      <c r="D62" s="67" t="s">
         <v>213</v>
       </c>
-      <c r="E62" s="66" t="s">
+      <c r="E62" s="70" t="s">
         <v>56</v>
       </c>
-      <c r="F62" s="64" t="s">
+      <c r="F62" s="67" t="s">
         <v>9</v>
       </c>
       <c r="G62" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="H62" s="70"/>
-    </row>
-    <row r="63" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="H62" s="73"/>
+    </row>
+    <row r="63" spans="3:8">
       <c r="C63" s="68"/>
       <c r="D63" s="68"/>
-      <c r="E63" s="69"/>
+      <c r="E63" s="71"/>
       <c r="F63" s="68"/>
       <c r="G63" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="H63" s="71"/>
-    </row>
-    <row r="64" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="H63" s="74"/>
+    </row>
+    <row r="64" spans="3:8">
       <c r="C64" s="68"/>
       <c r="D64" s="68"/>
-      <c r="E64" s="69"/>
+      <c r="E64" s="71"/>
       <c r="F64" s="68"/>
       <c r="G64" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="H64" s="71"/>
-    </row>
-    <row r="65" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C65" s="65"/>
-      <c r="D65" s="65"/>
-      <c r="E65" s="67"/>
-      <c r="F65" s="65"/>
+      <c r="H64" s="74"/>
+    </row>
+    <row r="65" spans="3:8">
+      <c r="C65" s="69"/>
+      <c r="D65" s="69"/>
+      <c r="E65" s="72"/>
+      <c r="F65" s="69"/>
       <c r="G65" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="H65" s="72"/>
-    </row>
-    <row r="66" spans="3:8" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H65" s="75"/>
+    </row>
+    <row r="66" spans="3:8" ht="54.75" customHeight="1">
       <c r="C66" s="30">
         <v>38</v>
       </c>
@@ -3281,55 +3282,55 @@
       <c r="G66" s="24"/>
       <c r="H66" s="22"/>
     </row>
-    <row r="67" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C67" s="64">
+    <row r="67" spans="3:8">
+      <c r="C67" s="67">
         <v>39</v>
       </c>
-      <c r="D67" s="64" t="s">
+      <c r="D67" s="67" t="s">
         <v>217</v>
       </c>
-      <c r="E67" s="66" t="s">
+      <c r="E67" s="70" t="s">
         <v>214</v>
       </c>
-      <c r="F67" s="64" t="s">
+      <c r="F67" s="67" t="s">
         <v>9</v>
       </c>
       <c r="G67" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="H67" s="70"/>
-    </row>
-    <row r="68" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="H67" s="73"/>
+    </row>
+    <row r="68" spans="3:8">
       <c r="C68" s="68"/>
       <c r="D68" s="68"/>
-      <c r="E68" s="69"/>
+      <c r="E68" s="71"/>
       <c r="F68" s="68"/>
       <c r="G68" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="H68" s="71"/>
-    </row>
-    <row r="69" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="H68" s="74"/>
+    </row>
+    <row r="69" spans="3:8">
       <c r="C69" s="68"/>
       <c r="D69" s="68"/>
-      <c r="E69" s="69"/>
+      <c r="E69" s="71"/>
       <c r="F69" s="68"/>
       <c r="G69" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="H69" s="71"/>
-    </row>
-    <row r="70" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C70" s="65"/>
-      <c r="D70" s="65"/>
-      <c r="E70" s="67"/>
-      <c r="F70" s="65"/>
+      <c r="H69" s="74"/>
+    </row>
+    <row r="70" spans="3:8">
+      <c r="C70" s="69"/>
+      <c r="D70" s="69"/>
+      <c r="E70" s="72"/>
+      <c r="F70" s="69"/>
       <c r="G70" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="H70" s="72"/>
-    </row>
-    <row r="71" spans="3:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H70" s="75"/>
+    </row>
+    <row r="71" spans="3:8" ht="20.100000000000001" customHeight="1">
       <c r="C71" s="5">
         <v>40</v>
       </c>
@@ -3342,12 +3343,12 @@
       <c r="F71" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="G71" s="53" t="s">
+      <c r="G71" s="52" t="s">
         <v>272</v>
       </c>
       <c r="H71" s="12"/>
     </row>
-    <row r="72" spans="3:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="3:8" ht="20.100000000000001" customHeight="1">
       <c r="C72" s="5">
         <v>41</v>
       </c>
@@ -3365,7 +3366,7 @@
       </c>
       <c r="H72" s="12"/>
     </row>
-    <row r="73" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="3:8">
       <c r="C73" s="5">
         <v>42</v>
       </c>
@@ -3383,7 +3384,7 @@
       </c>
       <c r="H73" s="12"/>
     </row>
-    <row r="74" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="3:8">
       <c r="C74" s="5">
         <v>43</v>
       </c>
@@ -3401,7 +3402,7 @@
       </c>
       <c r="H74" s="12"/>
     </row>
-    <row r="75" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="3:8">
       <c r="C75" s="5">
         <v>44</v>
       </c>
@@ -3419,7 +3420,7 @@
       </c>
       <c r="H75" s="12"/>
     </row>
-    <row r="76" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="3:8">
       <c r="C76" s="5">
         <v>45</v>
       </c>
@@ -3437,7 +3438,7 @@
       </c>
       <c r="H76" s="12"/>
     </row>
-    <row r="77" spans="3:8" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="77" spans="3:8" ht="40.5">
       <c r="C77" s="5">
         <v>46</v>
       </c>
@@ -3455,7 +3456,7 @@
       </c>
       <c r="H77" s="12"/>
     </row>
-    <row r="78" spans="3:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="3:8" ht="19.5" customHeight="1">
       <c r="C78" s="5">
         <v>47</v>
       </c>
@@ -3473,46 +3474,11 @@
       </c>
       <c r="H78" s="12"/>
     </row>
-    <row r="79" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="3:8">
       <c r="D79" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="C46:C49"/>
-    <mergeCell ref="D46:D49"/>
-    <mergeCell ref="E46:E49"/>
-    <mergeCell ref="F46:F49"/>
-    <mergeCell ref="H46:H49"/>
-    <mergeCell ref="C42:C45"/>
-    <mergeCell ref="D42:D45"/>
-    <mergeCell ref="E42:E45"/>
-    <mergeCell ref="F42:F45"/>
-    <mergeCell ref="H42:H45"/>
-    <mergeCell ref="C54:C57"/>
-    <mergeCell ref="D54:D57"/>
-    <mergeCell ref="E54:E57"/>
-    <mergeCell ref="F54:F57"/>
-    <mergeCell ref="H54:H57"/>
-    <mergeCell ref="C50:C53"/>
-    <mergeCell ref="D50:D53"/>
-    <mergeCell ref="E50:E53"/>
-    <mergeCell ref="F50:F53"/>
-    <mergeCell ref="H50:H53"/>
-    <mergeCell ref="C62:C65"/>
-    <mergeCell ref="D62:D65"/>
-    <mergeCell ref="E62:E65"/>
-    <mergeCell ref="F62:F65"/>
-    <mergeCell ref="H62:H65"/>
-    <mergeCell ref="C58:C61"/>
-    <mergeCell ref="D58:D61"/>
-    <mergeCell ref="E58:E61"/>
-    <mergeCell ref="F58:F61"/>
-    <mergeCell ref="H58:H61"/>
-    <mergeCell ref="C67:C70"/>
-    <mergeCell ref="D67:D70"/>
-    <mergeCell ref="E67:E70"/>
-    <mergeCell ref="F67:F70"/>
-    <mergeCell ref="H67:H70"/>
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="D11:D12"/>
     <mergeCell ref="E11:E12"/>
@@ -3525,6 +3491,41 @@
     <mergeCell ref="D9:D10"/>
     <mergeCell ref="E9:E10"/>
     <mergeCell ref="F9:F10"/>
+    <mergeCell ref="C67:C70"/>
+    <mergeCell ref="D67:D70"/>
+    <mergeCell ref="E67:E70"/>
+    <mergeCell ref="F67:F70"/>
+    <mergeCell ref="H67:H70"/>
+    <mergeCell ref="C58:C61"/>
+    <mergeCell ref="D58:D61"/>
+    <mergeCell ref="E58:E61"/>
+    <mergeCell ref="F58:F61"/>
+    <mergeCell ref="H58:H61"/>
+    <mergeCell ref="C62:C65"/>
+    <mergeCell ref="D62:D65"/>
+    <mergeCell ref="E62:E65"/>
+    <mergeCell ref="F62:F65"/>
+    <mergeCell ref="H62:H65"/>
+    <mergeCell ref="C50:C53"/>
+    <mergeCell ref="D50:D53"/>
+    <mergeCell ref="E50:E53"/>
+    <mergeCell ref="F50:F53"/>
+    <mergeCell ref="H50:H53"/>
+    <mergeCell ref="C54:C57"/>
+    <mergeCell ref="D54:D57"/>
+    <mergeCell ref="E54:E57"/>
+    <mergeCell ref="F54:F57"/>
+    <mergeCell ref="H54:H57"/>
+    <mergeCell ref="C42:C45"/>
+    <mergeCell ref="D42:D45"/>
+    <mergeCell ref="E42:E45"/>
+    <mergeCell ref="F42:F45"/>
+    <mergeCell ref="H42:H45"/>
+    <mergeCell ref="C46:C49"/>
+    <mergeCell ref="D46:D49"/>
+    <mergeCell ref="E46:E49"/>
+    <mergeCell ref="F46:F49"/>
+    <mergeCell ref="H46:H49"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3540,20 +3541,20 @@
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="7" max="7" width="25.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.44140625" customWidth="1"/>
-    <col min="9" max="9" width="33.109375" customWidth="1"/>
-    <col min="10" max="10" width="12.6640625" customWidth="1"/>
+    <col min="7" max="7" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" customWidth="1"/>
+    <col min="9" max="9" width="33.140625" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="5:10">
       <c r="E4" s="1" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="6" spans="5:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="5:10" ht="19.5" customHeight="1">
       <c r="E6" s="16" t="s">
         <v>5</v>
       </c>
@@ -3573,7 +3574,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="5:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="5:10" ht="24" customHeight="1">
       <c r="E7" s="4">
         <v>1</v>
       </c>
@@ -3591,7 +3592,7 @@
       </c>
       <c r="J7" s="12"/>
     </row>
-    <row r="8" spans="5:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="5:10" ht="24" customHeight="1">
       <c r="E8" s="4">
         <v>2</v>
       </c>
@@ -3609,7 +3610,7 @@
       </c>
       <c r="J8" s="12"/>
     </row>
-    <row r="9" spans="5:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="5:10" ht="24" customHeight="1">
       <c r="E9" s="4">
         <v>3</v>
       </c>
@@ -3627,7 +3628,7 @@
       </c>
       <c r="J9" s="12"/>
     </row>
-    <row r="10" spans="5:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="5:10" ht="24" customHeight="1">
       <c r="E10" s="4">
         <v>4</v>
       </c>
@@ -3645,7 +3646,7 @@
       </c>
       <c r="J10" s="12"/>
     </row>
-    <row r="11" spans="5:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="5:10" ht="24" customHeight="1">
       <c r="E11" s="4">
         <v>5</v>
       </c>
@@ -3663,7 +3664,7 @@
       </c>
       <c r="J11" s="12"/>
     </row>
-    <row r="12" spans="5:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="5:10" ht="24" customHeight="1">
       <c r="E12" s="4">
         <v>6</v>
       </c>
@@ -3681,7 +3682,7 @@
       </c>
       <c r="J12" s="12"/>
     </row>
-    <row r="13" spans="5:10" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="5:10" ht="63" customHeight="1">
       <c r="E13" s="4">
         <v>7</v>
       </c>
@@ -3699,7 +3700,7 @@
       </c>
       <c r="J13" s="12"/>
     </row>
-    <row r="14" spans="5:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="5:10" ht="24" customHeight="1">
       <c r="E14" s="4">
         <v>8</v>
       </c>
@@ -3732,20 +3733,20 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="7" max="7" width="26" customWidth="1"/>
-    <col min="8" max="8" width="18.88671875" customWidth="1"/>
-    <col min="9" max="9" width="35.6640625" customWidth="1"/>
-    <col min="10" max="10" width="15.6640625" customWidth="1"/>
+    <col min="8" max="8" width="18.85546875" customWidth="1"/>
+    <col min="9" max="9" width="35.7109375" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="5:10">
       <c r="E5" s="1" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="7" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="5:10">
       <c r="E7" s="16" t="s">
         <v>5</v>
       </c>
@@ -3765,8 +3766,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="5:10" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E8" s="45">
+    <row r="8" spans="5:10" ht="24.95" customHeight="1">
+      <c r="E8" s="44">
         <v>1</v>
       </c>
       <c r="F8" s="28" t="s">
@@ -3783,8 +3784,8 @@
       </c>
       <c r="J8" s="12"/>
     </row>
-    <row r="9" spans="5:10" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E9" s="45">
+    <row r="9" spans="5:10" ht="24.95" customHeight="1">
+      <c r="E9" s="44">
         <v>2</v>
       </c>
       <c r="F9" s="28" t="s">
@@ -3801,8 +3802,8 @@
       </c>
       <c r="J9" s="12"/>
     </row>
-    <row r="10" spans="5:10" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E10" s="45">
+    <row r="10" spans="5:10" ht="24.95" customHeight="1">
+      <c r="E10" s="44">
         <v>3</v>
       </c>
       <c r="F10" s="28" t="s">
@@ -3819,8 +3820,8 @@
       </c>
       <c r="J10" s="12"/>
     </row>
-    <row r="11" spans="5:10" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E11" s="45">
+    <row r="11" spans="5:10" ht="24.95" customHeight="1">
+      <c r="E11" s="44">
         <v>4</v>
       </c>
       <c r="F11" s="28" t="s">
@@ -3837,8 +3838,8 @@
       </c>
       <c r="J11" s="12"/>
     </row>
-    <row r="12" spans="5:10" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E12" s="45">
+    <row r="12" spans="5:10" ht="24.95" customHeight="1">
+      <c r="E12" s="44">
         <v>5</v>
       </c>
       <c r="F12" s="28" t="s">
@@ -3855,8 +3856,8 @@
       </c>
       <c r="J12" s="12"/>
     </row>
-    <row r="13" spans="5:10" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E13" s="45">
+    <row r="13" spans="5:10" ht="24.95" customHeight="1">
+      <c r="E13" s="44">
         <v>6</v>
       </c>
       <c r="F13" s="28" t="s">
@@ -3873,8 +3874,8 @@
       </c>
       <c r="J13" s="12"/>
     </row>
-    <row r="14" spans="5:10" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="E14" s="45">
+    <row r="14" spans="5:10" ht="40.5">
+      <c r="E14" s="44">
         <v>7</v>
       </c>
       <c r="F14" s="28" t="s">
@@ -3891,8 +3892,8 @@
       </c>
       <c r="J14" s="12"/>
     </row>
-    <row r="15" spans="5:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E15" s="45">
+    <row r="15" spans="5:10" ht="35.25" customHeight="1">
+      <c r="E15" s="44">
         <v>8</v>
       </c>
       <c r="F15" s="28" t="s">
@@ -3907,7 +3908,7 @@
       </c>
       <c r="J15" s="12"/>
     </row>
-    <row r="16" spans="5:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="5:10" ht="20.100000000000001" customHeight="1">
       <c r="E16" s="4">
         <v>9</v>
       </c>
@@ -3925,7 +3926,7 @@
       </c>
       <c r="J16" s="12"/>
     </row>
-    <row r="17" spans="5:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="5:10" ht="20.100000000000001" customHeight="1">
       <c r="E17" s="4">
         <v>10</v>
       </c>
@@ -3943,7 +3944,7 @@
       </c>
       <c r="J17" s="12"/>
     </row>
-    <row r="18" spans="5:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="5:10" ht="20.100000000000001" customHeight="1">
       <c r="E18" s="4">
         <v>11</v>
       </c>
@@ -3961,7 +3962,7 @@
       </c>
       <c r="J18" s="12"/>
     </row>
-    <row r="19" spans="5:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="5:10" ht="20.100000000000001" customHeight="1">
       <c r="E19" s="4">
         <v>12</v>
       </c>
@@ -3979,7 +3980,7 @@
       </c>
       <c r="J19" s="12"/>
     </row>
-    <row r="20" spans="5:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="5:10" ht="20.100000000000001" customHeight="1">
       <c r="E20" s="4">
         <v>13</v>
       </c>
@@ -3997,7 +3998,7 @@
       </c>
       <c r="J20" s="12"/>
     </row>
-    <row r="21" spans="5:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="5:10" ht="20.100000000000001" customHeight="1">
       <c r="E21" s="4">
         <v>14</v>
       </c>
@@ -4015,7 +4016,7 @@
       </c>
       <c r="J21" s="12"/>
     </row>
-    <row r="22" spans="5:10" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="5:10" ht="45.75" customHeight="1">
       <c r="E22" s="4">
         <v>15</v>
       </c>
@@ -4033,7 +4034,7 @@
       </c>
       <c r="J22" s="12"/>
     </row>
-    <row r="23" spans="5:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="5:10" ht="20.100000000000001" customHeight="1">
       <c r="E23" s="4">
         <v>16</v>
       </c>
@@ -4066,15 +4067,15 @@
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="15.109375" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" customWidth="1"/>
     <col min="6" max="6" width="18" customWidth="1"/>
     <col min="7" max="7" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:7">
       <c r="C5" s="13" t="s">
         <v>14</v>
       </c>
@@ -4088,7 +4089,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:7">
       <c r="C6" s="13">
         <v>0</v>
       </c>
@@ -4102,7 +4103,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:7">
       <c r="C7" s="14">
         <v>1</v>
       </c>
@@ -4116,7 +4117,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:7">
       <c r="C8" s="14">
         <v>2</v>
       </c>
@@ -4130,7 +4131,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:7">
       <c r="C9" s="14">
         <v>3</v>
       </c>
@@ -4138,7 +4139,7 @@
         <v>9600</v>
       </c>
     </row>
-    <row r="10" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:7">
       <c r="C10" s="14">
         <v>4</v>
       </c>
@@ -4146,7 +4147,7 @@
         <v>19200</v>
       </c>
     </row>
-    <row r="11" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:7">
       <c r="C11" s="14">
         <v>5</v>
       </c>
@@ -4154,7 +4155,7 @@
         <v>38400</v>
       </c>
     </row>
-    <row r="12" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:7">
       <c r="C12" s="14">
         <v>6</v>
       </c>
@@ -4162,7 +4163,7 @@
         <v>57600</v>
       </c>
     </row>
-    <row r="13" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:7">
       <c r="C13" s="14">
         <v>7</v>
       </c>
@@ -4180,18 +4181,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="D2:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="38" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="4:6">
       <c r="D2" s="32" t="s">
         <v>249</v>
       </c>
@@ -4202,7 +4203,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="3" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="4:6">
       <c r="D3" s="35">
         <v>43642</v>
       </c>
@@ -4213,7 +4214,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="4" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="4:6">
       <c r="D4" s="38">
         <v>43731</v>
       </c>
@@ -4224,7 +4225,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="5" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="4:6">
       <c r="D5" s="38">
         <v>43821</v>
       </c>
@@ -4235,15 +4236,15 @@
         <v>270</v>
       </c>
     </row>
-    <row r="6" spans="4:6" ht="29.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="4:6" ht="29.45" customHeight="1">
       <c r="D6" s="38">
         <v>44020</v>
       </c>
       <c r="E6" s="39" t="s">
+        <v>274</v>
+      </c>
+      <c r="F6" s="53" t="s">
         <v>275</v>
-      </c>
-      <c r="F6" s="73" t="s">
-        <v>276</v>
       </c>
     </row>
   </sheetData>

</xml_diff>